<commit_message>
update new trying marimekko chart
</commit_message>
<xml_diff>
--- a/data/_out/stat-file-out.xlsx
+++ b/data/_out/stat-file-out.xlsx
@@ -22,19 +22,19 @@
     <t>total</t>
   </si>
   <si>
-    <t>in-dev</t>
-  </si>
-  <si>
-    <t>completed</t>
+    <t>open</t>
+  </si>
+  <si>
+    <t>closed</t>
   </si>
   <si>
     <t>month-label</t>
   </si>
   <si>
-    <t>% in-dev</t>
-  </si>
-  <si>
-    <t>% completed</t>
+    <t>% open</t>
+  </si>
+  <si>
+    <t>% closed</t>
   </si>
   <si>
     <t>width</t>

</xml_diff>